<commit_message>
Added variable field input interpreter
</commit_message>
<xml_diff>
--- a/DataMan/Records/static/generic-template.xlsx
+++ b/DataMan/Records/static/generic-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M McCown\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M McCown\SCS\DataMan\Records\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B29466E-05FE-4F66-8FA2-1B8CF9E4828F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C220E2-455A-4CEE-ACCC-5CEE172DF69C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="264" yWindow="540" windowWidth="13380" windowHeight="11304" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="396" windowWidth="12384" windowHeight="11304" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="141">
   <si>
     <t>Species</t>
   </si>
@@ -701,9 +701,6 @@
   </si>
   <si>
     <t>File status:</t>
-  </si>
-  <si>
-    <t>File Hash:</t>
   </si>
   <si>
     <t>Storage Location</t>
@@ -1236,6 +1233,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1257,7 +1255,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1862,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:H2"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1880,16 +1877,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="77"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="45" t="s">
         <v>88</v>
       </c>
@@ -1898,18 +1895,18 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="76" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
       <c r="I2" s="46" t="s">
         <v>0</v>
       </c>
@@ -1918,16 +1915,16 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
       <c r="I3" s="48" t="s">
         <v>115</v>
       </c>
@@ -1936,16 +1933,16 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
       <c r="I4" s="50" t="s">
         <v>116</v>
       </c>
@@ -1954,14 +1951,14 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="79"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
       <c r="I5" s="48" t="s">
         <v>1</v>
       </c>
@@ -1970,30 +1967,30 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="79"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
       <c r="I6" s="50" t="s">
         <v>24</v>
       </c>
       <c r="J6" s="52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="79"/>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
+      <c r="A7" s="80"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
       <c r="I7" s="48" t="s">
         <v>2</v>
       </c>
@@ -2002,14 +1999,14 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="79"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
       <c r="I8" s="50" t="s">
         <v>5</v>
       </c>
@@ -2018,16 +2015,16 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="75" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="74"/>
+      <c r="A9" s="76" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="76"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="75"/>
       <c r="I9" s="48" t="s">
         <v>3</v>
       </c>
@@ -2091,7 +2088,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -2110,7 +2107,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -2129,7 +2126,7 @@
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="70" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -2407,13 +2404,13 @@
         <v>113</v>
       </c>
       <c r="I31" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="K31" s="11" t="s">
         <v>126</v>
-      </c>
-      <c r="J31" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="L31" s="11" t="s">
         <v>120</v>
@@ -2446,13 +2443,13 @@
         <v>43466</v>
       </c>
       <c r="I32" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J32" s="62" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K32" s="65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L32" s="62"/>
       <c r="M32" s="62"/>
@@ -2483,7 +2480,7 @@
         <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E34">
         <v>7</v>
@@ -2498,13 +2495,13 @@
         <v>43510</v>
       </c>
       <c r="I34" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="J34" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="J34" s="62" t="s">
+      <c r="K34" s="65" t="s">
         <v>136</v>
-      </c>
-      <c r="K34" s="65" t="s">
-        <v>137</v>
       </c>
       <c r="L34" s="62"/>
       <c r="M34" s="62"/>
@@ -2516,8 +2513,8 @@
       <c r="B35" s="5">
         <v>0</v>
       </c>
-      <c r="C35" s="80" t="s">
-        <v>141</v>
+      <c r="C35" s="73" t="s">
+        <v>140</v>
       </c>
       <c r="D35" s="16">
         <v>2</v>
@@ -3045,8 +3042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3155,7 +3152,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="55" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -3325,7 +3322,7 @@
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="60"/>
+      <c r="A9" s="56"/>
       <c r="B9">
         <v>8</v>
       </c>
@@ -3358,9 +3355,6 @@
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="58" t="s">
-        <v>122</v>
-      </c>
       <c r="B10">
         <v>9</v>
       </c>
@@ -3393,7 +3387,6 @@
       <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="56"/>
       <c r="B11">
         <v>10</v>
       </c>
@@ -3426,6 +3419,9 @@
       <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="55" t="s">
+        <v>133</v>
+      </c>
       <c r="B12">
         <v>11</v>
       </c>
@@ -3458,6 +3454,7 @@
       <c r="J12" s="16"/>
     </row>
     <row r="13" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="56"/>
       <c r="B13">
         <v>12</v>
       </c>
@@ -3490,9 +3487,6 @@
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="55" t="s">
-        <v>134</v>
-      </c>
       <c r="B14">
         <v>13</v>
       </c>
@@ -3525,7 +3519,6 @@
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="56"/>
       <c r="B15">
         <v>14</v>
       </c>
@@ -4097,6 +4090,9 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
       <c r="B34" t="s">
         <v>45</v>
       </c>
@@ -4161,9 +4157,6 @@
       <c r="J35" s="16"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>48</v>
-      </c>
       <c r="B36" t="s">
         <v>47</v>
       </c>

</xml_diff>